<commit_message>
changed silk on display board
</commit_message>
<xml_diff>
--- a/Project Outputs for WordStorm Display/BOM/Bill of Materials-WordStorm Display.xlsx
+++ b/Project Outputs for WordStorm Display/BOM/Bill of Materials-WordStorm Display.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\WordStorm Display\Project Outputs for WordStorm Display\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F287B10D-6D57-40DE-A020-B3D4EC1D23AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8F974C5-C681-40B9-B78D-A939D4C36687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{566DC5B9-ED43-4011-8264-B45ADC4CDE90}"/>
+    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{6E47B7EA-180F-4EFB-BB9B-0564D91B0F1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WordStorm Dis" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE737699-13C8-4CEB-B0B9-986CF7E513AA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5084B4F3-40BA-4110-AB34-B61A111BAE5D}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
changed hole size from 5mm to 4mm
also shrank annular ring to 6mm.
</commit_message>
<xml_diff>
--- a/Project Outputs for WordStorm Display/BOM/Bill of Materials-WordStorm Display.xlsx
+++ b/Project Outputs for WordStorm Display/BOM/Bill of Materials-WordStorm Display.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\WordStorm Display\Project Outputs for WordStorm Display\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8F974C5-C681-40B9-B78D-A939D4C36687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{80B8D1D1-5637-4077-97D6-193D49B999C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="1485" windowWidth="21600" windowHeight="13065" xr2:uid="{6E47B7EA-180F-4EFB-BB9B-0564D91B0F1A}"/>
+    <workbookView xWindow="3615" yWindow="2775" windowWidth="21600" windowHeight="13065" xr2:uid="{31C2E91D-9EA5-40CF-96C3-FFEA0F438101}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-WordStorm Dis" sheetId="1" r:id="rId1"/>
@@ -581,7 +581,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5084B4F3-40BA-4110-AB34-B61A111BAE5D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0BCB3AB-D242-4D69-BA74-D57C32EAEB73}">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>